<commit_message>
huge change for balance
</commit_message>
<xml_diff>
--- a/src/main/resources/fgo/localization/cards_noble.xlsx
+++ b/src/main/resources/fgo/localization/cards_noble.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,43 +410,52 @@
         <v>牌名</v>
       </c>
       <c r="C1" t="str">
-        <v>稀有度</v>
+        <v>类型</v>
       </c>
       <c r="D1" t="str">
-        <v>类型</v>
+        <v>目标</v>
       </c>
       <c r="E1" t="str">
-        <v>目标</v>
+        <v>费用</v>
       </c>
       <c r="F1" t="str">
-        <v>费用</v>
+        <v>描述</v>
       </c>
       <c r="G1" t="str">
-        <v>描述</v>
+        <v>伤害值</v>
       </c>
       <c r="H1" t="str">
-        <v>伤害值</v>
+        <v>格挡值</v>
       </c>
       <c r="I1" t="str">
-        <v>格挡值</v>
+        <v>特殊值</v>
       </c>
       <c r="J1" t="str">
-        <v>特殊值</v>
+        <v>宝具值</v>
       </c>
       <c r="K1" t="str">
+        <v>暴击星</v>
+      </c>
+      <c r="L1" t="str">
         <v>费用+</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>强化版描述</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>伤害值+</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>格挡值+</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>特殊值+</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>宝具值+</v>
+      </c>
+      <c r="R1" t="str">
+        <v>暴击星+</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
@@ -457,33 +466,29 @@
         <v>环抱着你的希望之星</v>
       </c>
       <c r="C2" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D2" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E2" t="str">
         <v>SELF</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str" xml:space="preserve">
-        <v xml:space="preserve">获得2点 力量 。 
- 移除所有负面 状态 。 
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="str" xml:space="preserve">
+        <v xml:space="preserve">获得3点 力量 。 
  获得 !M! 次 fgo:肃正防御 。 </v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="O2">
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="P2">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" xml:space="preserve">
       <c r="A3" t="str">
         <v>BeautifulJourney</v>
       </c>
@@ -491,37 +496,29 @@
         <v>超越边界的存在</v>
       </c>
       <c r="C3" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D3" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E3" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <v>对所有敌人造成 !D! 点伤害。每有一名敌人，就获得 !NP! % fgo:宝具值 。</v>
-      </c>
-      <c r="H3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str" xml:space="preserve">
+        <v xml:space="preserve"> fgo:宝具值获取提升 ，回合结束时移除。 
+ 对所有敌人造成 !D! 点伤害。每有一名敌人，就获得 !NP! % fgo:宝具值 。</v>
+      </c>
+      <c r="G3">
         <v>24</v>
       </c>
-      <c r="J3">
-        <v>20</v>
-      </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-      <c r="M3">
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="O3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
+    </row>
+    <row r="4">
       <c r="A4" t="str">
         <v>Failnaught</v>
       </c>
@@ -529,29 +526,25 @@
         <v>痛哭幻奏</v>
       </c>
       <c r="C4" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D4" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E4" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="str" xml:space="preserve">
-        <v xml:space="preserve">去除敌人的 格挡 和 人工制品 。 
- 造成 !D! 点伤害。</v>
-      </c>
-      <c r="H4">
-        <v>32</v>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4">
-        <v>40</v>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="str">
+        <v>使敌人失去 !D! 点生命。</v>
+      </c>
+      <c r="G4">
+        <v>48</v>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4">
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -562,27 +555,24 @@
         <v>无元剑制</v>
       </c>
       <c r="C5" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D5" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E5" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
         <v>对所有敌人造成 !D! 点伤害6次，失去所有 力量 。</v>
       </c>
-      <c r="H5">
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5">
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5">
         <v>5</v>
       </c>
     </row>
@@ -594,28 +584,25 @@
         <v>伪·军神五兵</v>
       </c>
       <c r="C6" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D6" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E6" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
         <v>对所有敌人造成 !D! 点伤害 !M! 次，给予 !M! 层 虚弱 。</v>
       </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6">
-        <v>8</v>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6">
+        <v>6</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
@@ -626,29 +613,32 @@
         <v>赠予新娘的纺车</v>
       </c>
       <c r="C7" t="str">
-        <v>SPECIAL</v>
+        <v>SKILL</v>
       </c>
       <c r="D7" t="str">
-        <v>SKILL</v>
-      </c>
-      <c r="E7" t="str">
         <v>SELF</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str" xml:space="preserve">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str" xml:space="preserve">
         <v xml:space="preserve">{@@}获得 {!M!|repeat= [E]} 。 
  获得 !Star! 颗 fgo:暴击星 。</v>
       </c>
-      <c r="J7">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="O7">
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="P7">
         <v>4</v>
+      </c>
+      <c r="R7">
+        <v>20</v>
       </c>
     </row>
     <row r="8" xml:space="preserve">
@@ -659,29 +649,32 @@
         <v>狂暴少女狼</v>
       </c>
       <c r="C8" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D8" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E8" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str" xml:space="preserve">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str" xml:space="preserve">
         <v xml:space="preserve">使敌人失去 !D! 点生命。 
  给予 !M! 层 易伤 。</v>
       </c>
-      <c r="H8">
-        <v>30</v>
-      </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-      <c r="M8">
-        <v>40</v>
+      <c r="G8">
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8">
+        <v>34</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -692,27 +685,24 @@
         <v>选定之枪</v>
       </c>
       <c r="C9" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D9" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E9" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
         <v xml:space="preserve"> fgo:无敌贯通 。对所有敌人造成 !D! 点伤害，移除 *坚不可摧 。</v>
       </c>
-      <c r="H9">
+      <c r="G9">
         <v>24</v>
       </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-      <c r="M9">
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9">
         <v>30</v>
       </c>
     </row>
@@ -724,28 +714,25 @@
         <v>轮转胜利之剑</v>
       </c>
       <c r="C10" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D10" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E10" t="str">
         <v>SELF</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str" xml:space="preserve">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str" xml:space="preserve">
         <v xml:space="preserve">获得 fgo:阳光照射 3回合。 
  获得 !M! 点 活力 。</v>
       </c>
-      <c r="J10">
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="L10" t="str">
-        <v/>
-      </c>
-      <c r="O10">
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="P10">
         <v>4</v>
       </c>
     </row>
@@ -757,29 +744,26 @@
         <v>缚锁全断·过重湖光</v>
       </c>
       <c r="C11" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D11" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E11" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str" xml:space="preserve">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str" xml:space="preserve">
         <v xml:space="preserve"> fgo:宝具值获取提升 。 
  去除敌人的 格挡 值。 
  造成 !D! 点伤害。</v>
       </c>
-      <c r="H11">
+      <c r="G11">
         <v>30</v>
       </c>
-      <c r="L11" t="str">
-        <v/>
-      </c>
-      <c r="M11">
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11">
         <v>38</v>
       </c>
     </row>
@@ -791,37 +775,34 @@
         <v>永世隔绝的理想乡</v>
       </c>
       <c r="C12" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D12" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E12" t="str">
         <v>SELF</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str" xml:space="preserve">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="str" xml:space="preserve">
         <v xml:space="preserve">在你的回合开始时 
  获得 !B! 点 格挡 ， 
  获得 !NP! % fgo:宝具值 ， 
  获得 !Star! 颗 fgo:暴击星 。</v>
       </c>
-      <c r="I12">
+      <c r="H12">
         <v>5</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>5</v>
       </c>
-      <c r="L12" t="str">
-        <v/>
-      </c>
-      <c r="N12">
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="O12">
         <v>8</v>
       </c>
-      <c r="O12">
-        <v>5</v>
+      <c r="R12">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -832,27 +813,24 @@
         <v>这是常识</v>
       </c>
       <c r="C13" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D13" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E13" t="str">
         <v>SELF</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="str">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="str">
         <v>在你的回合开始时，有 格挡 的敌人失去等于其 格挡 的生命并且给予其 !M! 层 易伤 。</v>
       </c>
-      <c r="J13">
+      <c r="I13">
         <v>2</v>
       </c>
-      <c r="L13" t="str">
-        <v/>
-      </c>
-      <c r="O13">
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="P13">
         <v>4</v>
       </c>
     </row>
@@ -864,29 +842,26 @@
         <v>鹦鹉螺的大冲角</v>
       </c>
       <c r="C14" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D14" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E14" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F14">
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="G14" t="str" xml:space="preserve">
+      <c r="F14" t="str" xml:space="preserve">
         <v xml:space="preserve">造成 !D! 点伤害。 
  fgo:水边 ：伤害提高50%。 
  fgo:水边 ：获得 [E] 。</v>
       </c>
-      <c r="H14">
+      <c r="G14">
         <v>40</v>
       </c>
-      <c r="L14" t="str">
-        <v/>
-      </c>
-      <c r="M14">
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14">
         <v>52</v>
       </c>
     </row>
@@ -898,29 +873,26 @@
         <v>与彼方同坠的梦之瞳眸</v>
       </c>
       <c r="C15" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D15" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E15" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="str" xml:space="preserve">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害，失去2点 力量 ， 
  给予 !M! 层 无实体 。 
  获得 !M! 层 无实体 。</v>
       </c>
-      <c r="H15">
+      <c r="G15">
         <v>25</v>
       </c>
-      <c r="L15" t="str">
-        <v/>
-      </c>
-      <c r="M15">
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15">
         <v>32</v>
       </c>
     </row>
@@ -932,34 +904,31 @@
         <v>业已无法抵达的理想乡</v>
       </c>
       <c r="C16" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D16" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E16" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="str" xml:space="preserve">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str" xml:space="preserve">
         <v xml:space="preserve">{@@}对所有敌人造成 !D! 点伤害3次。 
  你打出的下{!M!|1=一|@= !M! }张 fgo:宝具牌 将被打出两次。</v>
       </c>
-      <c r="H16">
+      <c r="G16">
         <v>8</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="str">
-        <v/>
-      </c>
-      <c r="M16">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16">
         <v>10</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>2</v>
       </c>
     </row>
@@ -971,28 +940,25 @@
         <v>捕食日轮之角</v>
       </c>
       <c r="C17" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D17" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E17" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="str" xml:space="preserve">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害5次。 
  获得 !M! 层 *多层护甲 。</v>
       </c>
-      <c r="H17">
+      <c r="G17">
         <v>5</v>
       </c>
-      <c r="L17" t="str">
-        <v/>
-      </c>
-      <c r="M17">
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17">
         <v>7</v>
       </c>
     </row>
@@ -1004,30 +970,27 @@
         <v>痛幻哭奏</v>
       </c>
       <c r="C18" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D18" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E18" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="str" xml:space="preserve">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="str" xml:space="preserve">
         <v xml:space="preserve">造成 !D! 点伤害。 
  敌人每有一层 fgo:诅呪 伤害就提高10%。 
  给予 !M! 层 fgo:诅呪 。 
  将敌人的 fgo:诅呪 层数翻倍。</v>
       </c>
-      <c r="H18">
+      <c r="G18">
         <v>30</v>
       </c>
-      <c r="L18" t="str">
-        <v/>
-      </c>
-      <c r="M18">
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18">
         <v>38</v>
       </c>
     </row>
@@ -1039,29 +1002,26 @@
         <v>尚未知晓的无垢湖光</v>
       </c>
       <c r="C19" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D19" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E19" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="str" xml:space="preserve">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="str" xml:space="preserve">
         <v xml:space="preserve">造成 !D! 点伤害。 
  获得 !M! 层 fgo:黄金律 。 
  将一张 *光之地平线+ 放入你的抽牌堆。</v>
       </c>
-      <c r="H19">
+      <c r="G19">
         <v>32</v>
       </c>
-      <c r="L19" t="str">
-        <v/>
-      </c>
-      <c r="M19">
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19">
         <v>40</v>
       </c>
     </row>
@@ -1073,28 +1033,25 @@
         <v>无人知晓的无垢搏动</v>
       </c>
       <c r="C20" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D20" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E20" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="str" xml:space="preserve">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str" xml:space="preserve">
         <v xml:space="preserve">所有敌人失去 !D! 点生命。 
  获得 !Star! 颗 fgo:暴击星 。</v>
       </c>
-      <c r="H20">
+      <c r="G20">
         <v>27</v>
       </c>
-      <c r="L20" t="str">
-        <v/>
-      </c>
-      <c r="M20">
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20">
         <v>35</v>
       </c>
     </row>
@@ -1106,29 +1063,35 @@
         <v>79式掷祸大社</v>
       </c>
       <c r="C21" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D21" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E21" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="str" xml:space="preserve">
-        <v xml:space="preserve">对所有敌人造成 !D! 点伤害8次。 
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="str" xml:space="preserve">
+        <v xml:space="preserve">获得 1 点 力量 。 
+ 你的回合结束时，失去 1 点 力量 。 
+ 对所有敌人造成 !D! 点伤害。 
+ 减少敌人多段攻击1段。 
  获得 !NP! % fgo:宝具值 。</v>
       </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="L21" t="str">
-        <v/>
-      </c>
-      <c r="M21">
-        <v>4</v>
+      <c r="G21">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="M21" t="str">
+        <v/>
+      </c>
+      <c r="N21">
+        <v>32</v>
+      </c>
+      <c r="Q21">
+        <v>30</v>
       </c>
     </row>
     <row r="22" xml:space="preserve">
@@ -1139,29 +1102,32 @@
         <v>誓约胜利之剑</v>
       </c>
       <c r="C22" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D22" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E22" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="str" xml:space="preserve">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害。 
  获得 !NP! % fgo:宝具值 。</v>
       </c>
-      <c r="H22">
+      <c r="G22">
         <v>25</v>
       </c>
-      <c r="L22" t="str">
-        <v/>
-      </c>
-      <c r="M22">
+      <c r="J22">
+        <v>20</v>
+      </c>
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22">
         <v>32</v>
+      </c>
+      <c r="Q22">
+        <v>50</v>
       </c>
     </row>
     <row r="23" xml:space="preserve">
@@ -1172,34 +1138,31 @@
         <v>拟似展开／人理之础</v>
       </c>
       <c r="C23" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D23" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E23" t="str">
         <v>SELF</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="str" xml:space="preserve">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="str" xml:space="preserve">
         <v xml:space="preserve">获得 !B! 点 格挡 。 
  在这个回合受到的攻击伤害降低 !M! %。</v>
       </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
       <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
         <v>10</v>
       </c>
-      <c r="L23" t="str">
-        <v/>
-      </c>
-      <c r="N23">
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="O23">
         <v>7</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>20</v>
       </c>
     </row>
@@ -1211,35 +1174,32 @@
         <v>已然遥远的理想之城</v>
       </c>
       <c r="C24" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D24" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E24" t="str">
         <v>SELF</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="str" xml:space="preserve">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="str" xml:space="preserve">
         <v xml:space="preserve">获得 !B! 点 格挡 。 
  获得2点 力量 。 
  在这个回合受到的攻击伤害降低 !M! %。</v>
       </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
       <c r="I24">
-        <v>5</v>
-      </c>
-      <c r="J24">
         <v>10</v>
       </c>
-      <c r="L24" t="str">
-        <v/>
-      </c>
-      <c r="N24">
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="O24">
         <v>12</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>30</v>
       </c>
     </row>
@@ -1251,35 +1211,26 @@
         <v>构筑希望的人理之盾</v>
       </c>
       <c r="C25" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D25" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E25" t="str">
         <v>SELF</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="str" xml:space="preserve">
-        <v xml:space="preserve">获得1层 人工制品 ， !B! fgo:金属化 ， 3层 力量 ， !M! % fgo:伤害减免 。 
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="str" xml:space="preserve">
+        <v xml:space="preserve">获得1层 人工制品 ， !${modID}:metal! fgo:金属化 ， 3层 力量 ， !M! % fgo:伤害减免 。 
  获得30% fgo:宝具威力 。 
   fgo:迦勒底的圣骑士 。</v>
       </c>
       <c r="I25">
-        <v>5</v>
-      </c>
-      <c r="J25">
         <v>30</v>
       </c>
-      <c r="L25" t="str">
-        <v/>
-      </c>
-      <c r="N25">
-        <v>10</v>
-      </c>
-      <c r="O25">
+      <c r="M25" t="str">
+        <v/>
+      </c>
+      <c r="P25">
         <v>50</v>
       </c>
     </row>
@@ -1291,29 +1242,27 @@
         <v>明证希望的人理之剑</v>
       </c>
       <c r="C26" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D26" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E26" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="str" xml:space="preserve">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="str" xml:space="preserve">
         <v xml:space="preserve">fgo:无敌贯通 。 
  给予所有敌人 !M! 层易伤 。 
- 对所有敌人造成 !D! 点伤害。</v>
-      </c>
-      <c r="H26">
+ 对所有敌人造成 !D! 点伤害。 
+ 移除BOSS以外敌人所有增益。</v>
+      </c>
+      <c r="G26">
         <v>20</v>
       </c>
-      <c r="L26" t="str">
-        <v/>
-      </c>
-      <c r="M26">
+      <c r="M26" t="str">
+        <v/>
+      </c>
+      <c r="N26">
         <v>40</v>
       </c>
     </row>
@@ -1325,21 +1274,18 @@
         <v>虎啊，煌煌燎燃</v>
       </c>
       <c r="C27" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D27" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E27" t="str">
         <v>SELF</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="str">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="str">
         <v>在你没有 *羽翼之靴 时，获得 *羽翼之靴 。</v>
       </c>
-      <c r="L27" t="str">
+      <c r="M27" t="str">
         <v/>
       </c>
     </row>
@@ -1351,29 +1297,26 @@
         <v>星月夜</v>
       </c>
       <c r="C28" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D28" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E28" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F28">
+      <c r="E28">
         <v>2</v>
       </c>
-      <c r="G28" t="str" xml:space="preserve">
+      <c r="F28" t="str" xml:space="preserve">
         <v xml:space="preserve">给予所有敌人3层 fgo:恐怖 (60%概率)。 
- 获得 !M! 点 力量 和50% fgo:暴击威力 。 
+ 获得 !M! 点 力量 和 !${modID}:CriticalDamage! % fgo:暴击威力 。 
  每回合获得10颗 fgo:暴击星 。</v>
       </c>
-      <c r="J28">
+      <c r="I28">
         <v>3</v>
       </c>
-      <c r="L28" t="str">
-        <v/>
-      </c>
-      <c r="O28">
+      <c r="M28" t="str">
+        <v/>
+      </c>
+      <c r="P28">
         <v>5</v>
       </c>
     </row>
@@ -1385,27 +1328,24 @@
         <v>斩剜战神之剑</v>
       </c>
       <c r="C29" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D29" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E29" t="str">
         <v>SELF</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" t="str">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="str">
         <v>在本回合，每当你被攻击时，对攻击者造成 !D! 点伤害，并且你获得4颗 fgo:暴击星 。</v>
       </c>
-      <c r="H29">
+      <c r="G29">
         <v>15</v>
       </c>
-      <c r="L29" t="str">
-        <v/>
-      </c>
-      <c r="M29">
+      <c r="M29" t="str">
+        <v/>
+      </c>
+      <c r="N29">
         <v>20</v>
       </c>
     </row>
@@ -1417,28 +1357,25 @@
         <v>星，自宇宙降临</v>
       </c>
       <c r="C30" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D30" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E30" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="str" xml:space="preserve">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害5次。 
  获得 !Star! 颗 fgo:暴击星 。</v>
       </c>
-      <c r="H30">
+      <c r="G30">
         <v>6</v>
       </c>
-      <c r="L30" t="str">
-        <v/>
-      </c>
-      <c r="M30">
+      <c r="M30" t="str">
+        <v/>
+      </c>
+      <c r="N30">
         <v>8</v>
       </c>
     </row>
@@ -1450,28 +1387,25 @@
         <v>裁定归灭之回剑</v>
       </c>
       <c r="C31" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D31" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E31" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="str" xml:space="preserve">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害5次。 
  额外造成所有敌人总负面 状态 种类的伤害。</v>
       </c>
-      <c r="H31">
+      <c r="G31">
         <v>5</v>
       </c>
-      <c r="L31" t="str">
-        <v/>
-      </c>
-      <c r="M31">
+      <c r="M31" t="str">
+        <v/>
+      </c>
+      <c r="N31">
         <v>6</v>
       </c>
     </row>
@@ -1483,27 +1417,24 @@
         <v>灵峰踏抱冥府之鞴</v>
       </c>
       <c r="C32" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D32" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E32" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="str">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="str">
         <v>对所有敌人造成 !D! 点伤害，没有 *飞行 状态的敌人额外失去10%最大生命。</v>
       </c>
-      <c r="H32">
+      <c r="G32">
         <v>26</v>
       </c>
-      <c r="L32" t="str">
-        <v/>
-      </c>
-      <c r="M32">
+      <c r="M32" t="str">
+        <v/>
+      </c>
+      <c r="N32">
         <v>34</v>
       </c>
     </row>
@@ -1515,23 +1446,26 @@
         <v>冥镜宝典</v>
       </c>
       <c r="C33" t="str">
-        <v>SPECIAL</v>
+        <v>SKILL</v>
       </c>
       <c r="D33" t="str">
-        <v>SKILL</v>
-      </c>
-      <c r="E33" t="str">
         <v>SELF</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="str" xml:space="preserve">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="str" xml:space="preserve">
         <v xml:space="preserve">选择一张已 消耗 的牌，将其 升级 并且放入你的手牌。 
  所有 *爪牙 敌人死亡，每只获得 !NP! % fgo:宝具值 。</v>
       </c>
-      <c r="L33" t="str">
-        <v/>
+      <c r="J33">
+        <v>25</v>
+      </c>
+      <c r="M33" t="str">
+        <v/>
+      </c>
+      <c r="Q33">
+        <v>50</v>
       </c>
     </row>
     <row r="34" xml:space="preserve">
@@ -1542,28 +1476,25 @@
         <v>祈祷之弓</v>
       </c>
       <c r="C34" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D34" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E34" t="str">
         <v>ENEMY</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="str" xml:space="preserve">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="str" xml:space="preserve">
         <v xml:space="preserve">造成 !D! 点伤害。 
  如果敌人有 中毒 状态 ，则再次造成 !D! 点伤害。</v>
       </c>
-      <c r="H34">
+      <c r="G34">
         <v>25</v>
       </c>
-      <c r="L34" t="str">
-        <v/>
-      </c>
-      <c r="M34">
+      <c r="M34" t="str">
+        <v/>
+      </c>
+      <c r="N34">
         <v>30</v>
       </c>
     </row>
@@ -1575,27 +1506,24 @@
         <v>无限剑制</v>
       </c>
       <c r="C35" t="str">
-        <v>SPECIAL</v>
+        <v>POWER</v>
       </c>
       <c r="D35" t="str">
-        <v>POWER</v>
-      </c>
-      <c r="E35" t="str">
         <v>SELF</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="str">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
         <v>{@@}在你的回合开始时，增加{!M!|1=一|@= !M! }张随机攻击牌到你的手牌。它{!M!|1=|@=们}在本回合耗能变为0，打出后 消耗 。</v>
       </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="L35" t="str">
-        <v/>
-      </c>
-      <c r="O35">
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+      <c r="P35">
         <v>2</v>
       </c>
     </row>
@@ -1607,27 +1535,24 @@
         <v>天地乖离开辟之星</v>
       </c>
       <c r="C36" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D36" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E36" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="str">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="str">
         <v>对所有敌人造成 !D! 点伤害。</v>
       </c>
-      <c r="H36">
+      <c r="G36">
         <v>32</v>
       </c>
-      <c r="L36" t="str">
-        <v/>
-      </c>
-      <c r="M36">
+      <c r="M36" t="str">
+        <v/>
+      </c>
+      <c r="N36">
         <v>40</v>
       </c>
     </row>
@@ -1639,28 +1564,25 @@
         <v>水天日光天照八野镇石</v>
       </c>
       <c r="C37" t="str">
-        <v>SPECIAL</v>
+        <v>SKILL</v>
       </c>
       <c r="D37" t="str">
-        <v>SKILL</v>
-      </c>
-      <c r="E37" t="str">
         <v>SELF</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="str" xml:space="preserve">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="str" xml:space="preserve">
         <v xml:space="preserve">你手牌中的所有牌在本回合的耗能减少1点。 
  获得 !M! % fgo:宝具值 。</v>
       </c>
-      <c r="J37">
-        <v>35</v>
-      </c>
-      <c r="L37" t="str">
-        <v/>
-      </c>
-      <c r="O37">
+      <c r="I37">
+        <v>25</v>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+      <c r="P37">
         <v>50</v>
       </c>
     </row>
@@ -1672,42 +1594,69 @@
         <v>青色美丽的尼罗河</v>
       </c>
       <c r="C38" t="str">
-        <v>SPECIAL</v>
+        <v>ATTACK</v>
       </c>
       <c r="D38" t="str">
-        <v>ATTACK</v>
-      </c>
-      <c r="E38" t="str">
         <v>ALL_ENEMY</v>
       </c>
-      <c r="F38">
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="G38" t="str" xml:space="preserve">
+      <c r="F38" t="str" xml:space="preserve">
         <v xml:space="preserve">对所有敌人造成 !D! 点伤害。 
  给予 3 层 易伤 。 
  如果敌人的生命值小于等于 !M! 点，则将其生命值变为0。 
  获得 fgo:水边 。</v>
       </c>
-      <c r="H38">
+      <c r="G38">
         <v>35</v>
       </c>
-      <c r="J38">
+      <c r="I38">
         <v>10</v>
       </c>
-      <c r="L38" t="str">
-        <v/>
-      </c>
-      <c r="M38">
+      <c r="M38" t="str">
+        <v/>
+      </c>
+      <c r="N38">
         <v>45</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>15</v>
+      </c>
+    </row>
+    <row r="39" xml:space="preserve">
+      <c r="A39" t="str">
+        <v>CodeOriginalSin</v>
+      </c>
+      <c r="B39" t="str">
+        <v>第七圣典·断罪死</v>
+      </c>
+      <c r="C39" t="str">
+        <v>ATTACK</v>
+      </c>
+      <c r="D39" t="str">
+        <v>ENEMY</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="str" xml:space="preserve">
+        <v xml:space="preserve">使敌人失去 !D! 点生命。 
+ 获得 !NP! % fgo:宝具值 。</v>
+      </c>
+      <c r="G39">
+        <v>32</v>
+      </c>
+      <c r="M39" t="str">
+        <v/>
+      </c>
+      <c r="N39">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>